<commit_message>
update DelBay data summary
</commit_message>
<xml_diff>
--- a/DelBay_summary/DelBay19_summary_final.xlsx
+++ b/DelBay_summary/DelBay19_summary_final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/cornell/Backup/Ryan_workplace/DelBay_adult/summary/DelBay/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HG/Documents/HG/Github/HG_Code_Bay/DelBay_summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4639EFE-501B-7549-996A-57F4D0F8BB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D53A3F9-C2E1-DE4F-89D3-09EC83428403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33200" yWindow="5420" windowWidth="48960" windowHeight="15800" activeTab="1" xr2:uid="{73E658AF-ED84-4A4A-B677-E5A3A024EED6}"/>
+    <workbookView xWindow="28820" yWindow="4100" windowWidth="48960" windowHeight="21400" activeTab="1" xr2:uid="{73E658AF-ED84-4A4A-B677-E5A3A024EED6}"/>
   </bookViews>
   <sheets>
     <sheet name="Caption" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2764" uniqueCount="912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2766" uniqueCount="914">
   <si>
     <t>Sample</t>
   </si>
@@ -2775,6 +2775,12 @@
   </si>
   <si>
     <t>Proportion of reference genome covered</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Del19 challenge only</t>
   </si>
 </sst>
 </file>
@@ -2782,8 +2788,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000000000"/>
+    <numFmt numFmtId="172" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -2898,7 +2904,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2923,13 +2929,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3496,10 +3508,10 @@
   <dimension ref="A1:AF508"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K308" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1:G1048576"/>
+      <selection pane="bottomRight" activeCell="AB333" sqref="AB333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.3984375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3523,12 +3535,12 @@
     <col min="24" max="24" width="19.3984375" style="4" customWidth="1"/>
     <col min="25" max="25" width="21.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.59765625" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.3984375" style="2"/>
+    <col min="27" max="27" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="33" max="16384" width="12.3984375" style="1"/>
   </cols>
   <sheetData>
@@ -13818,7 +13830,7 @@
       </c>
     </row>
     <row r="113" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A113" s="18" t="s">
+      <c r="A113" s="17" t="s">
         <v>286</v>
       </c>
       <c r="B113" s="1" t="s">
@@ -18928,7 +18940,7 @@
       </c>
     </row>
     <row r="168" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A168" s="18" t="s">
+      <c r="A168" s="17" t="s">
         <v>421</v>
       </c>
       <c r="B168" s="1" t="s">
@@ -24984,7 +24996,7 @@
       </c>
     </row>
     <row r="236" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A236" s="18" t="s">
+      <c r="A236" s="17" t="s">
         <v>577</v>
       </c>
       <c r="B236" s="1" t="s">
@@ -26078,7 +26090,7 @@
       </c>
     </row>
     <row r="247" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A247" s="18" t="s">
+      <c r="A247" s="17" t="s">
         <v>607</v>
       </c>
       <c r="B247" s="1" t="s">
@@ -26666,7 +26678,7 @@
       </c>
     </row>
     <row r="253" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A253" s="18" t="s">
+      <c r="A253" s="17" t="s">
         <v>623</v>
       </c>
       <c r="B253" s="1" t="s">
@@ -31052,7 +31064,7 @@
       </c>
     </row>
     <row r="298" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A298" s="18" t="s">
+      <c r="A298" s="17" t="s">
         <v>745</v>
       </c>
       <c r="B298" s="1" t="s">
@@ -31934,7 +31946,7 @@
       </c>
     </row>
     <row r="307" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A307" s="18" t="s">
+      <c r="A307" s="17" t="s">
         <v>772</v>
       </c>
       <c r="B307" s="1" t="s">
@@ -34122,7 +34134,7 @@
       </c>
     </row>
     <row r="329" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A329" s="18" t="s">
+      <c r="A329" s="17" t="s">
         <v>844</v>
       </c>
       <c r="B329" s="1" t="s">
@@ -34498,82 +34510,90 @@
       </c>
     </row>
     <row r="333" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="L333" s="1">
-        <f>MEDIAN(L2:L332)</f>
-        <v>11706668</v>
-      </c>
-      <c r="Z333" s="1">
-        <f>MEDIAN(Z236:Z332)</f>
-        <v>527741717</v>
-      </c>
-      <c r="AA333" s="4"/>
-      <c r="AB333" s="16">
-        <f>MEDIAN(AB2:AB332)</f>
-        <v>0.86559508515506001</v>
-      </c>
-      <c r="AC333" s="16">
-        <f t="shared" ref="AC333:AD333" si="27">MEDIAN(AC2:AC332)</f>
-        <v>1.48927174196909</v>
-      </c>
-      <c r="AD333" s="16">
-        <f t="shared" si="27"/>
-        <v>2.3915191344497702</v>
-      </c>
-      <c r="AE333" s="16">
-        <f>MEDIAN(AE2:AE332)</f>
-        <v>0.55600204414863696</v>
-      </c>
-      <c r="AF333" s="16">
-        <f t="shared" ref="AF333" si="28">MEDIAN(AF2:AF332)</f>
-        <v>0.362487288772875</v>
-      </c>
-    </row>
-    <row r="334" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="L334" s="15">
+      <c r="A333" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="L333" s="15">
         <f>AVERAGE(L2:L332)</f>
         <v>13042430.193353474</v>
       </c>
+      <c r="M333" s="1">
+        <f t="shared" ref="M333:O333" si="27">AVERAGE(M2:M332)</f>
+        <v>1966952789.0392749</v>
+      </c>
+      <c r="N333" s="1">
+        <f t="shared" si="27"/>
+        <v>1908658297.8731117</v>
+      </c>
+      <c r="O333" s="1">
+        <f t="shared" si="27"/>
+        <v>1592854584.9154079</v>
+      </c>
+      <c r="V333" s="3">
+        <f>AVERAGE(V2:V332)</f>
+        <v>1273134605.6072507</v>
+      </c>
+      <c r="W333" s="3">
+        <f t="shared" ref="W333:AE333" si="28">AVERAGE(W2:W332)</f>
+        <v>699421825.95166159</v>
+      </c>
+      <c r="X333" s="4">
+        <f t="shared" si="28"/>
+        <v>0.5484801811931399</v>
+      </c>
+      <c r="Y333" s="18">
+        <f t="shared" si="28"/>
+        <v>637483067.30211484</v>
+      </c>
+      <c r="Z333" s="18">
+        <f t="shared" si="28"/>
+        <v>626975850.84290028</v>
+      </c>
+      <c r="AA333" s="19">
+        <f t="shared" si="28"/>
+        <v>0.31832275586378378</v>
+      </c>
+      <c r="AB333" s="19">
+        <f t="shared" si="28"/>
+        <v>0.9144101776938236</v>
+      </c>
+      <c r="AC333" s="19">
+        <f t="shared" si="28"/>
+        <v>1.5533632097833328</v>
+      </c>
+      <c r="AD333" s="19">
+        <f t="shared" si="28"/>
+        <v>2.4948270130442829</v>
+      </c>
+      <c r="AE333" s="19">
+        <f t="shared" si="28"/>
+        <v>0.64720320074696502</v>
+      </c>
+      <c r="AF333" s="19">
+        <f>AVERAGE(AF2:AF332)</f>
+        <v>0.35331544491811412</v>
+      </c>
+    </row>
+    <row r="334" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="L334" s="15"/>
       <c r="AA334" s="4"/>
-      <c r="AB334" s="2">
-        <f>STDEV(AB2:AB332)</f>
-        <v>0.3813155504446461</v>
-      </c>
-      <c r="AD334" s="2">
-        <f>STDEV(AD2:AD332)</f>
-        <v>0.68427778145349816</v>
-      </c>
     </row>
     <row r="335" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="L335" s="1">
-        <f>MEDIAN(L236:L332)</f>
-        <v>10578712</v>
-      </c>
       <c r="AA335" s="4"/>
-      <c r="AB335" s="17">
-        <f>MEDIAN(AB236:AB332)</f>
-        <v>0.76811020762886795</v>
-      </c>
-      <c r="AC335" s="17"/>
-      <c r="AD335" s="17">
-        <f>MEDIAN(AD236:AD332)</f>
-        <v>2.2268747290993698</v>
-      </c>
+      <c r="AB335" s="16" t="s">
+        <v>913</v>
+      </c>
+      <c r="AC335" s="16"/>
+      <c r="AD335" s="16"/>
     </row>
     <row r="336" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="L336" s="1">
-        <f>AVERAGE(L236:L332)</f>
-        <v>10829740.288659794</v>
-      </c>
       <c r="AA336" s="4"/>
-      <c r="AB336" s="17">
+      <c r="AB336" s="20">
         <f>AVERAGE(AB236:AB332)</f>
         <v>0.77753117480443534</v>
       </c>
-      <c r="AC336" s="17"/>
-      <c r="AD336" s="17">
-        <f>AVERAGE(AD236:AD332)</f>
-        <v>2.2506381584133899</v>
-      </c>
+      <c r="AC336" s="16"/>
+      <c r="AD336" s="16"/>
     </row>
     <row r="337" spans="1:27" x14ac:dyDescent="0.2">
       <c r="AA337" s="4"/>

</xml_diff>